<commit_message>
update seeder and module
</commit_message>
<xml_diff>
--- a/database/seeders/excel/branch_niise.xlsx
+++ b/database/seeders/excel/branch_niise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71FB9D8-41C6-4521-AD0B-031B6DC96D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C43CF2-D342-4C56-BB7D-9446CC16B3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$48</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="95">
   <si>
     <t>Johor</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Bahagian Visa, Pas dan Permit</t>
   </si>
   <si>
-    <t xml:space="preserve">Bahagian Keselamatan dan Pasport </t>
-  </si>
-  <si>
     <t>Jabatan Imigresen Malaysia, 
 No. 17, Tingkat 3 (Tower A) Menara Ikhlas, Persiaran Perdana, Presint 3, 
 62100 Putrajaya</t>
@@ -341,9 +338,6 @@
   </si>
   <si>
     <t>Bahagian Pengurusan Depot dan Tahanan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bahagian Perisikan dan Operasi Khas </t>
   </si>
   <si>
     <t>Bahagian Atipsom dan AMLA</t>
@@ -793,10 +787,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="B46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,10 +1266,10 @@
         <v>65</v>
       </c>
       <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -1286,7 +1280,7 @@
         <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>71</v>
@@ -1300,7 +1294,7 @@
         <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>71</v>
@@ -1314,7 +1308,7 @@
         <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>71</v>
@@ -1328,7 +1322,7 @@
         <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>71</v>
@@ -1342,7 +1336,7 @@
         <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>71</v>
@@ -1356,7 +1350,7 @@
         <v>65</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>71</v>
@@ -1370,7 +1364,7 @@
         <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>71</v>
@@ -1384,7 +1378,7 @@
         <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>71</v>
@@ -1398,7 +1392,7 @@
         <v>65</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1408,8 +1402,8 @@
       <c r="A45" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>73</v>
+      <c r="B45" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1419,109 +1413,54 @@
       <c r="A46" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>74</v>
+      <c r="B46" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>65</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>88</v>
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>65</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D52" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>93</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D53" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>96</v>
-      </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D53" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:D48" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
         <filter val="Cawangan"/>

</xml_diff>